<commit_message>
fixed png rescaling issues
</commit_message>
<xml_diff>
--- a/Area_weight_table.xlsx
+++ b/Area_weight_table.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="295">
   <si>
     <t xml:space="preserve">Wall-Farm</t>
   </si>
@@ -838,25 +838,211 @@
     <t xml:space="preserve">Add unusable images (due to bad masks) with cropping too</t>
   </si>
   <si>
+    <t xml:space="preserve">Reservoir_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cropped_by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant area(pixels)_image1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerry</t>
+  </si>
+  <si>
     <t xml:space="preserve">902.018, 136.447</t>
   </si>
   <si>
     <t xml:space="preserve">876.005, 136.447</t>
   </si>
   <si>
+    <t xml:space="preserve">Sushmita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">799.267, 544.785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800.567, 570.798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">808.371, 578.601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">808.371, 547.386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800.567, 611.118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800.567, 581.203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">583.55, 263.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">608.42, 263.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">565.224, 823.725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">536.424, 825.035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">611.042, 818.816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">587.478, 818.816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">635.385, 77.853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">660.098, 77.853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">712.123, 160.271 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">691.571, 161.571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">697.442, 745.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">697.442, 724.71</t>
+  </si>
+  <si>
     <t xml:space="preserve">839.587, 134.93</t>
   </si>
   <si>
     <t xml:space="preserve">814.874, 134.93</t>
   </si>
   <si>
+    <t xml:space="preserve">849.992, 65.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">826.58, 65.3235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">762.849, 98.663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">742.038, 98.663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">608.424, 785.325 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">587.478,785.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">580.933, 801.471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">559.987, 800.162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">302.096, 903.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">324.351, 898.344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">635.915, 818.336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">659.478, 817.027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">618.896, 837.973 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">643.769, 836.664</t>
+  </si>
+  <si>
+    <t xml:space="preserve">575.69, 536.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">575.69, 555.842</t>
+  </si>
+  <si>
+    <t xml:space="preserve">797.966, 73.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">820.077, 73.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">251.695, 88.735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">229.584, 88.735</t>
+  </si>
+  <si>
     <t xml:space="preserve">844.789, 95.9103</t>
   </si>
   <si>
     <t xml:space="preserve">818.776, 95.9103</t>
   </si>
   <si>
-    <t xml:space="preserve">Img 8994 not used because scale not clear</t>
+    <t xml:space="preserve">Img 8994 and 9112_2 not used because scale not clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">611.04, 759.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">628.06, 759.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9112_2 is the same as 9112 with dimensions changed for uniformity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">523.333, 859.071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">540.351, 857.762</t>
+  </si>
+  <si>
+    <t xml:space="preserve">596.642, 884.816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">616.278, 884.816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">521.277, 767.033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">537.006, 767.033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">489.296, 742.562</t>
+  </si>
+  <si>
+    <t xml:space="preserve">469.66, 742.562</t>
+  </si>
+  <si>
+    <t xml:space="preserve">768.051, 531.778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">766.751, 552.589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">554.751, 756.962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">537.733, 755.653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">663.405, 756.962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">645.078, 756.962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">524.642, 838.125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">540.351, 842.053</t>
   </si>
   <si>
     <t xml:space="preserve">812.293, 132.48</t>
@@ -865,190 +1051,16 @@
     <t xml:space="preserve">788.862, 131.179</t>
   </si>
   <si>
-    <t xml:space="preserve">635.385, 77.853</t>
-  </si>
-  <si>
-    <t xml:space="preserve">660.098, 77.853</t>
-  </si>
-  <si>
-    <t xml:space="preserve">849.992, 65.32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">826.58, 65.3235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">251.695, 88.735</t>
-  </si>
-  <si>
-    <t xml:space="preserve">229.584, 88.735</t>
-  </si>
-  <si>
     <t xml:space="preserve">969.651, 99.14</t>
   </si>
   <si>
     <t xml:space="preserve">942.338, 100.441</t>
   </si>
   <si>
-    <t xml:space="preserve">712.123, 160.271 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">691.571, 161.571</t>
-  </si>
-  <si>
-    <t xml:space="preserve">762.849, 98.663</t>
-  </si>
-  <si>
-    <t xml:space="preserve">742.038, 98.663</t>
-  </si>
-  <si>
-    <t xml:space="preserve">797.966, 73.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">820.077, 73.12</t>
-  </si>
-  <si>
     <t xml:space="preserve">667.33, 698.53</t>
   </si>
   <si>
     <t xml:space="preserve">668.64, 669.73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">697.442, 745.66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">697.442, 724.71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">575.69, 536.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">575.69, 555.842</t>
-  </si>
-  <si>
-    <t xml:space="preserve">583.55, 263.91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">608.42, 263.91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">565.224, 823.725</t>
-  </si>
-  <si>
-    <t xml:space="preserve">536.424, 825.035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">611.042, 818.816</t>
-  </si>
-  <si>
-    <t xml:space="preserve">587.478, 818.816</t>
-  </si>
-  <si>
-    <t xml:space="preserve">608.424, 785.325 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">587.478,785.325</t>
-  </si>
-  <si>
-    <t xml:space="preserve">580.933, 801.471</t>
-  </si>
-  <si>
-    <t xml:space="preserve">559.987, 800.162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">302.096, 903.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">324.351, 898.344</t>
-  </si>
-  <si>
-    <t xml:space="preserve">635.915, 818.336</t>
-  </si>
-  <si>
-    <t xml:space="preserve">659.478, 817.027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">618.896, 837.973 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">643.769, 836.664</t>
-  </si>
-  <si>
-    <t xml:space="preserve">611.04, 759.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">628.06, 759.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">523.333, 859.071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">540.351, 857.762</t>
-  </si>
-  <si>
-    <t xml:space="preserve">596.642, 884.816</t>
-  </si>
-  <si>
-    <t xml:space="preserve">616.278, 884.816</t>
-  </si>
-  <si>
-    <t xml:space="preserve">521.277, 767.033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">537.006, 767.033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">796.856, 290.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">796.856, 304.495</t>
-  </si>
-  <si>
-    <t xml:space="preserve">489.296, 742.562</t>
-  </si>
-  <si>
-    <t xml:space="preserve">469.66, 742.562</t>
-  </si>
-  <si>
-    <t xml:space="preserve">768.051, 531.778</t>
-  </si>
-  <si>
-    <t xml:space="preserve">766.751, 552.589</t>
-  </si>
-  <si>
-    <t xml:space="preserve">554.751, 756.962</t>
-  </si>
-  <si>
-    <t xml:space="preserve">537.733, 755.653</t>
-  </si>
-  <si>
-    <t xml:space="preserve">663.405, 756.962</t>
-  </si>
-  <si>
-    <t xml:space="preserve">645.078, 756.962</t>
-  </si>
-  <si>
-    <t xml:space="preserve">524.642, 838.125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">540.351, 842.053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">799.267, 544.785</t>
-  </si>
-  <si>
-    <t xml:space="preserve">800.567, 570.798</t>
-  </si>
-  <si>
-    <t xml:space="preserve">808.371, 578.601</t>
-  </si>
-  <si>
-    <t xml:space="preserve">808.371, 547.386</t>
-  </si>
-  <si>
-    <t xml:space="preserve">800.567, 611.118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">800.567, 581.203</t>
   </si>
 </sst>
 </file>
@@ -1718,9 +1730,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>226440</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1730,7 +1742,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4615920" y="298080"/>
-          <a:ext cx="6235920" cy="3774240"/>
+          <a:ext cx="6233760" cy="3772080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7076,9 +7088,9 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="B65" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="B62" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L70" activeCellId="0" sqref="L70"/>
+      <selection pane="bottomLeft" activeCell="H65" activeCellId="0" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10879,7 +10891,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11638,29 +11650,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M27" activeCellId="0" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="15.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>107</v>
@@ -11672,18 +11684,24 @@
         <v>204</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>209</v>
       </c>
     </row>
@@ -11700,220 +11718,257 @@
       <c r="D2" s="1" t="n">
         <v>47.13</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F2" s="65" t="n">
+        <v>244444</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>361.24</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="39" t="n">
+        <v>46.56</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F3" s="39" t="n">
+        <v>63976</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>360.68</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="39" t="n">
+        <v>27.93</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F4" s="39" t="n">
+        <v>49242</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>192.75</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="39" t="n">
+        <v>42.61</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F5" s="39" t="n">
+        <v>70322</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>301</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>46.8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="65" t="n">
+        <v>49748</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>307.08</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>34.96</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F7" s="65" t="n">
+        <v>67188</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>309.26</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>63.66</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F8" s="65" t="n">
+        <v>65455</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>451.79</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>8939</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>45.97</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>351.36</v>
-      </c>
-      <c r="F3" s="1" t="n">
+      <c r="C9" s="1" t="n">
+        <v>8960</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>31.48</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F9" s="65" t="n">
+        <v>151722</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>248.43</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>8940</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>53.55</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>343.89</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>8941</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>46.64</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>339.37</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="str">
-        <f aca="false">A2</f>
-        <v>C1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>8960</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>31.48</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>248.43</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="str">
-        <f aca="false">A3</f>
-        <v>C2</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>8961</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>86</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>478.73</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="str">
-        <f aca="false">A4</f>
-        <v>C3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>8962</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>63.77</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>386.03</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="str">
-        <f aca="false">A5</f>
-        <v>C4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>8978</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>24.96</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>261.31</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="str">
-        <f aca="false">A6</f>
-        <v>C1</v>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>216</v>
@@ -11924,239 +11979,290 @@
       <c r="D10" s="1" t="n">
         <v>94.56</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F10" s="65" t="n">
+        <v>256677</v>
+      </c>
+      <c r="G10" s="1" t="n">
         <v>605.26</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="str">
-        <f aca="false">A7</f>
-        <v>C2</v>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>216</v>
+        <v>151</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>8980</v>
+        <v>8993</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>139.25</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>599.88</v>
-      </c>
-      <c r="F11" s="1" t="n">
+        <v>132.12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F11" s="65" t="n">
+        <v>344126</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>784.06</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>240</v>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="str">
-        <f aca="false">A8</f>
-        <v>C3</v>
+      <c r="A12" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>216</v>
+        <v>93</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>8981</v>
+        <v>8939</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>86.15</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>498.76</v>
-      </c>
-      <c r="F12" s="1" t="n">
+        <v>45.97</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="65" t="n">
+        <v>214588</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>351.36</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>242</v>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="str">
-        <f aca="false">A9</f>
-        <v>C4</v>
+        <f aca="false">A12</f>
+        <v>C2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>151</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>8992</v>
+        <v>8961</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>46.28</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>314.33</v>
-      </c>
-      <c r="F13" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F13" s="65" t="n">
+        <v>262402</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>478.73</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>244</v>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="str">
-        <f aca="false">A10</f>
-        <v>C1</v>
+        <f aca="false">A13</f>
+        <v>C2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>151</v>
+        <v>216</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>8993</v>
+        <v>8980</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>132.12</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>784.06</v>
-      </c>
-      <c r="F14" s="1" t="n">
+        <v>139.25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F14" s="65" t="n">
+        <v>259807</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>599.88</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>246</v>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="str">
-        <f aca="false">A12</f>
-        <v>C3</v>
+      <c r="A15" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>8995</v>
+        <v>154</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>144.38</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>738.03</v>
-      </c>
-      <c r="F15" s="1" t="n">
+        <v>89.25</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F15" s="65" t="n">
+        <v>68077</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>592.84</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>248</v>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>46.8</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>80.43</v>
-      </c>
-      <c r="F16" s="1" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F16" s="65" t="n">
+        <v>53806</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>464.67</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>250</v>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>34.96</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>80.84</v>
-      </c>
-      <c r="F17" s="1" t="n">
+        <v>107.67</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F17" s="65" t="n">
+        <v>70478</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>516.36</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>252</v>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>217</v>
+        <v>170</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>63.66</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>117.88</v>
-      </c>
-      <c r="F18" s="1" t="n">
+        <v>93.24</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F18" s="65" t="n">
+        <v>69208</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>474.99</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>254</v>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12164,134 +12270,170 @@
         <v>91</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>89.25</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>155.17</v>
-      </c>
-      <c r="F19" s="1" t="n">
+        <v>119.88</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F19" s="65" t="n">
+        <v>71654</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>442.27</v>
+      </c>
+      <c r="H19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>91</v>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="str">
+        <f aca="false">A21</f>
+        <v>C3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>168</v>
+        <v>151</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>8995</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>99.7</v>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>122.16</v>
-      </c>
-      <c r="F20" s="1" t="n">
+        <v>144.38</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F20" s="65" t="n">
+        <v>284738</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>738.03</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>91</v>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="str">
+        <f aca="false">A22</f>
+        <v>C3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>169</v>
+        <v>216</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>8981</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>107.67</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>134.83</v>
-      </c>
-      <c r="F21" s="1" t="n">
+        <v>86.15</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F21" s="65" t="n">
+        <v>243843</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>498.76</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>91</v>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="str">
+        <f aca="false">A23</f>
+        <v>C3</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>8962</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>63.77</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F22" s="65" t="n">
+        <v>188728</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>386.03</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>93.24</v>
-      </c>
-      <c r="E22" s="1" t="n">
-        <v>124.27</v>
-      </c>
-      <c r="F22" s="1" t="n">
+      <c r="B23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>8940</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>53.55</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F23" s="65" t="n">
+        <v>232700</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>343.89</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>119.88</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>115.5</v>
-      </c>
-      <c r="F23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>264</v>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12307,18 +12449,27 @@
       <c r="D24" s="1" t="n">
         <v>180.83</v>
       </c>
-      <c r="E24" s="1" t="n">
-        <v>265.07</v>
-      </c>
-      <c r="F24" s="1" t="n">
+      <c r="E24" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F24" s="65" t="n">
+        <v>76787</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>1012.24</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>266</v>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12334,18 +12485,24 @@
       <c r="D25" s="1" t="n">
         <v>148.19</v>
       </c>
-      <c r="E25" s="1" t="n">
-        <v>218.66</v>
+      <c r="E25" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="F25" s="1" t="n">
+        <v>63700</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>832.15</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>268</v>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12361,18 +12518,24 @@
       <c r="D26" s="1" t="n">
         <v>135.95</v>
       </c>
-      <c r="E26" s="1" t="n">
-        <v>179.26</v>
+      <c r="E26" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="F26" s="1" t="n">
+        <v>69118</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>687.56</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>270</v>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12388,45 +12551,57 @@
       <c r="D27" s="1" t="n">
         <v>277.64</v>
       </c>
-      <c r="E27" s="1" t="n">
-        <v>344.86</v>
+      <c r="E27" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="F27" s="1" t="n">
+        <v>85318</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>1306.29</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>272</v>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>256.91</v>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>471</v>
-      </c>
-      <c r="F28" s="1" t="n">
+        <v>148.72</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F28" s="65" t="n">
+        <v>66662</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>661.59</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>274</v>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12434,26 +12609,32 @@
         <v>93</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>148.72</v>
-      </c>
-      <c r="E29" s="1" t="n">
-        <v>172.89</v>
+        <v>201</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="F29" s="1" t="n">
+        <v>69797</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>613.11</v>
+      </c>
+      <c r="H29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>276</v>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12461,26 +12642,32 @@
         <v>93</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="E30" s="1" t="n">
-        <v>160.53</v>
+        <v>202.24</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="F30" s="1" t="n">
+        <v>67755</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>888.13</v>
+      </c>
+      <c r="H30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>278</v>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12488,26 +12675,32 @@
         <v>93</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>202.24</v>
-      </c>
-      <c r="E31" s="1" t="n">
-        <v>232.57</v>
+        <v>187.28</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="F31" s="1" t="n">
+        <v>60209</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>684.15</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>280</v>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12515,133 +12708,149 @@
         <v>93</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>187.28</v>
-      </c>
-      <c r="E32" s="1" t="n">
-        <v>179.26</v>
+        <v>206.19</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="F32" s="1" t="n">
+        <v>60159</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>876.07</v>
+      </c>
+      <c r="H32" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="1"/>
+      <c r="J32" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>187</v>
+        <v>91</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>8941</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>206.19</v>
-      </c>
-      <c r="E33" s="1" t="n">
-        <v>229.44</v>
-      </c>
-      <c r="F33" s="1" t="n">
+        <v>46.64</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F33" s="65" t="n">
+        <v>186892</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>339.37</v>
+      </c>
+      <c r="H33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="65" t="s">
-        <v>164</v>
-      </c>
-      <c r="D34" s="39" t="n">
-        <v>46.56</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>94.31</v>
-      </c>
-      <c r="F34" s="0" t="n">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="str">
+        <f aca="false">A33</f>
+        <v>C4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>8978</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>24.96</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F34" s="65" t="n">
+        <v>195377</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>261.31</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H34" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="C35" s="65" t="s">
-        <v>159</v>
-      </c>
-      <c r="D35" s="39" t="n">
-        <v>27.93</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>50.54</v>
-      </c>
-      <c r="F35" s="0" t="n">
+      <c r="I34" s="1"/>
+      <c r="J34" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="str">
+        <f aca="false">A34</f>
+        <v>C4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>8992</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>46.28</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F35" s="65" t="n">
+        <v>261260</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>314.33</v>
+      </c>
+      <c r="H35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H35" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="65" t="s">
-        <v>162</v>
-      </c>
-      <c r="D36" s="39" t="n">
-        <v>42.61</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>78.58</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>290</v>
-      </c>
-    </row>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>